<commit_message>
added formats for the time based excel sheet
</commit_message>
<xml_diff>
--- a/Timebased-graph-data.xlsx
+++ b/Timebased-graph-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Data\Desktop\Major-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Data\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC1800D0-9EBD-44D0-AD0F-6ECDD2EAFABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4659D62F-785B-49F8-B757-60820240D01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C8D5C3D4-922A-48D2-BA21-B55B622E3E48}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t>Time based tests</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Type of Website</t>
+  </si>
+  <si>
+    <t>Real Estate website</t>
   </si>
 </sst>
 </file>
@@ -88,9 +94,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,156 +418,703 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ADB214-92B1-453C-ACC5-1479AC4E3929}">
-  <dimension ref="B3:D17"/>
+  <dimension ref="A3:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
       <c r="B7">
+        <v>1080</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>1080</v>
-      </c>
-      <c r="D7">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="M8" s="2">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="M9" s="2">
+        <v>3</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1247</v>
+      </c>
+      <c r="C10">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="M10" s="2">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>948</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="M12" s="2">
+        <v>6</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>881</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="M13" s="2">
+        <v>7</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1231</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="E14" s="2">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="2">
+        <v>8</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="M14" s="2">
+        <v>8</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>533</v>
+      </c>
+      <c r="C15">
+        <v>48</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="2">
+        <v>9</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="M15" s="2">
+        <v>9</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="2">
+        <v>10</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="M16" s="2">
+        <v>10</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>603.4</v>
+      </c>
+      <c r="C17">
+        <v>81.8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(F7:F16)/10</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(G7:G16)/10</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="2">
+        <f>SUM(J7:J16)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <f>SUM(K7:K16)/10</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="2">
+        <f>SUM(N7:N16)/10</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <f>SUM(O7:O16)/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="M27" s="2">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="M28" s="2">
+        <v>3</v>
+      </c>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="E29" s="2">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="2"/>
+      <c r="I29" s="2">
+        <v>4</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="M29" s="2">
+        <v>4</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="M30" s="2">
+        <v>5</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="E31" s="2">
+        <v>6</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="I31" s="2">
+        <v>6</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="M31" s="2">
+        <v>6</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="E32" s="2">
+        <v>7</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="I32" s="2">
+        <v>7</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="M32" s="2">
+        <v>7</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="E33" s="2">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="I33" s="2">
+        <v>8</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2"/>
+      <c r="M33" s="2">
+        <v>8</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>9</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="E34" s="2">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="I34" s="2">
+        <v>9</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="M34" s="2">
+        <v>9</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1247</v>
-      </c>
-      <c r="D10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>948</v>
-      </c>
-      <c r="D11">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>881</v>
-      </c>
-      <c r="D13">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1231</v>
-      </c>
-      <c r="D14">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <v>533</v>
-      </c>
-      <c r="D15">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="E35" s="2">
         <v>10</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>603.4</v>
-      </c>
-      <c r="D17">
-        <v>81.8</v>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="I35" s="2">
+        <v>10</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="M35" s="2">
+        <v>10</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <f>SUM(B26:B35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <f>SUM(C26:C35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="2">
+        <f>SUM(F26:F35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <f>SUM(G26:G35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="2">
+        <f>SUM(J26:J35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <f>SUM(K26:K35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="2">
+        <f>SUM(N26:N35)/10</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="2">
+        <f>SUM(O26:O35)/10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>